<commit_message>
adding bias resistor to anode
</commit_message>
<xml_diff>
--- a/output/sigsub_rev1_bom.xlsx
+++ b/output/sigsub_rev1_bom.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel2\projects\sigsub\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="19275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-sigsub" sheetId="1" r:id="rId1"/>
@@ -119,7 +114,7 @@
     <t>ZXM61N03F</t>
   </si>
   <si>
-    <t>R1, R2, R5, R6, R7, R8</t>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12</t>
   </si>
   <si>
     <t>Thick Film Resistor 47k +/-1% 0805</t>
@@ -165,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,13 +171,6 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -228,15 +216,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,9 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -529,7 +513,7 @@
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -557,68 +541,68 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>9</v>
@@ -626,22 +610,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>9</v>
@@ -649,22 +633,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>9</v>
@@ -672,75 +656,75 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F7" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>